<commit_message>
Update Temperate Forest Traits.xlsx
</commit_message>
<xml_diff>
--- a/Temperate Forest Traits.xlsx
+++ b/Temperate Forest Traits.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="265">
   <si>
     <t>Individual</t>
   </si>
@@ -1152,8 +1152,8 @@
   </sheetPr>
   <dimension ref="A1:L340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="137" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="137" workbookViewId="0">
+      <selection activeCell="F202" sqref="F202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2887,6 +2887,12 @@
       <c r="B160" s="1">
         <v>8</v>
       </c>
+      <c r="E160">
+        <v>81</v>
+      </c>
+      <c r="F160">
+        <v>62</v>
+      </c>
     </row>
     <row r="161" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
@@ -2895,6 +2901,12 @@
       <c r="B161" s="1">
         <v>8</v>
       </c>
+      <c r="E161">
+        <v>163</v>
+      </c>
+      <c r="F161">
+        <v>101</v>
+      </c>
     </row>
     <row r="162" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
@@ -2903,6 +2915,12 @@
       <c r="B162" s="1">
         <v>8</v>
       </c>
+      <c r="E162">
+        <v>87</v>
+      </c>
+      <c r="F162">
+        <v>81</v>
+      </c>
     </row>
     <row r="163" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
@@ -2911,6 +2929,12 @@
       <c r="B163" s="1">
         <v>8</v>
       </c>
+      <c r="E163">
+        <v>63</v>
+      </c>
+      <c r="F163">
+        <v>160</v>
+      </c>
     </row>
     <row r="164" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
@@ -2919,6 +2943,12 @@
       <c r="B164" s="1">
         <v>8</v>
       </c>
+      <c r="E164">
+        <v>109</v>
+      </c>
+      <c r="F164">
+        <v>130</v>
+      </c>
     </row>
     <row r="165" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
@@ -2927,6 +2957,12 @@
       <c r="B165" s="1">
         <v>8</v>
       </c>
+      <c r="E165">
+        <v>92</v>
+      </c>
+      <c r="F165">
+        <v>140</v>
+      </c>
     </row>
     <row r="166" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
@@ -2935,6 +2971,12 @@
       <c r="B166" s="1">
         <v>8</v>
       </c>
+      <c r="E166">
+        <v>125</v>
+      </c>
+      <c r="F166">
+        <v>111</v>
+      </c>
     </row>
     <row r="167" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
@@ -2943,6 +2985,12 @@
       <c r="B167" s="1">
         <v>8</v>
       </c>
+      <c r="E167">
+        <v>140</v>
+      </c>
+      <c r="F167">
+        <v>93</v>
+      </c>
     </row>
     <row r="168" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
@@ -2951,6 +2999,12 @@
       <c r="B168" s="1">
         <v>8</v>
       </c>
+      <c r="E168">
+        <v>55</v>
+      </c>
+      <c r="F168">
+        <v>85</v>
+      </c>
     </row>
     <row r="169" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
@@ -2973,6 +3027,12 @@
       <c r="B170" s="1">
         <v>8</v>
       </c>
+      <c r="E170">
+        <v>130</v>
+      </c>
+      <c r="F170">
+        <v>116</v>
+      </c>
     </row>
     <row r="171" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
@@ -2981,6 +3041,12 @@
       <c r="B171" s="1">
         <v>8</v>
       </c>
+      <c r="E171">
+        <v>90</v>
+      </c>
+      <c r="F171">
+        <v>51</v>
+      </c>
     </row>
     <row r="172" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
@@ -2989,6 +3055,12 @@
       <c r="B172" s="1">
         <v>8</v>
       </c>
+      <c r="E172">
+        <v>99</v>
+      </c>
+      <c r="F172">
+        <v>50</v>
+      </c>
     </row>
     <row r="173" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
@@ -2997,6 +3069,12 @@
       <c r="B173" s="1">
         <v>8</v>
       </c>
+      <c r="E173">
+        <v>105</v>
+      </c>
+      <c r="F173">
+        <v>63</v>
+      </c>
     </row>
     <row r="174" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
@@ -3019,6 +3097,12 @@
       <c r="B175" s="1">
         <v>8</v>
       </c>
+      <c r="E175">
+        <v>120</v>
+      </c>
+      <c r="F175">
+        <v>59</v>
+      </c>
     </row>
     <row r="176" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
@@ -3041,6 +3125,12 @@
       <c r="B177" s="1">
         <v>8</v>
       </c>
+      <c r="E177">
+        <v>111</v>
+      </c>
+      <c r="F177">
+        <v>81</v>
+      </c>
     </row>
     <row r="178" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
@@ -3049,6 +3139,12 @@
       <c r="B178" s="1">
         <v>8</v>
       </c>
+      <c r="E178">
+        <v>120</v>
+      </c>
+      <c r="F178">
+        <v>93</v>
+      </c>
     </row>
     <row r="179" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
@@ -3071,6 +3167,12 @@
       <c r="B180" s="1">
         <v>8</v>
       </c>
+      <c r="E180">
+        <v>91</v>
+      </c>
+      <c r="F180">
+        <v>43</v>
+      </c>
     </row>
     <row r="181" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
@@ -3079,6 +3181,12 @@
       <c r="B181" s="1">
         <v>8</v>
       </c>
+      <c r="E181">
+        <v>93</v>
+      </c>
+      <c r="F181">
+        <v>34</v>
+      </c>
     </row>
     <row r="182" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
@@ -3087,6 +3195,12 @@
       <c r="B182" s="1">
         <v>8</v>
       </c>
+      <c r="E182">
+        <v>110</v>
+      </c>
+      <c r="F182">
+        <v>53</v>
+      </c>
     </row>
     <row r="183" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
@@ -3123,6 +3237,9 @@
       <c r="B185" s="1">
         <v>8</v>
       </c>
+      <c r="E185">
+        <v>65</v>
+      </c>
     </row>
     <row r="186" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
@@ -3131,6 +3248,12 @@
       <c r="B186" s="1">
         <v>8</v>
       </c>
+      <c r="E186">
+        <v>105</v>
+      </c>
+      <c r="F186">
+        <v>120</v>
+      </c>
     </row>
     <row r="187" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
@@ -3139,6 +3262,12 @@
       <c r="B187" s="1">
         <v>8</v>
       </c>
+      <c r="E187">
+        <v>105</v>
+      </c>
+      <c r="F187">
+        <v>65</v>
+      </c>
     </row>
     <row r="188" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="1" t="s">
@@ -3147,6 +3276,12 @@
       <c r="B188" s="1">
         <v>8</v>
       </c>
+      <c r="E188">
+        <v>122</v>
+      </c>
+      <c r="F188">
+        <v>84</v>
+      </c>
     </row>
     <row r="189" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
@@ -3169,6 +3304,9 @@
       <c r="B190" s="1">
         <v>8</v>
       </c>
+      <c r="E190" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="191" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
@@ -3177,6 +3315,12 @@
       <c r="B191" s="1">
         <v>8</v>
       </c>
+      <c r="E191">
+        <v>120</v>
+      </c>
+      <c r="F191">
+        <v>64</v>
+      </c>
     </row>
     <row r="192" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
@@ -3185,6 +3329,12 @@
       <c r="B192" s="1">
         <v>8</v>
       </c>
+      <c r="E192">
+        <v>130</v>
+      </c>
+      <c r="F192">
+        <v>54</v>
+      </c>
     </row>
     <row r="193" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
@@ -3193,6 +3343,12 @@
       <c r="B193" s="1">
         <v>8</v>
       </c>
+      <c r="E193">
+        <v>105</v>
+      </c>
+      <c r="F193">
+        <v>60</v>
+      </c>
     </row>
     <row r="194" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
@@ -3201,6 +3357,12 @@
       <c r="B194" s="1">
         <v>8</v>
       </c>
+      <c r="E194">
+        <v>123</v>
+      </c>
+      <c r="F194">
+        <v>117</v>
+      </c>
     </row>
     <row r="195" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
@@ -3209,6 +3371,12 @@
       <c r="B195" s="1">
         <v>8</v>
       </c>
+      <c r="E195">
+        <v>115</v>
+      </c>
+      <c r="F195">
+        <v>55</v>
+      </c>
     </row>
     <row r="196" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
@@ -3217,6 +3385,12 @@
       <c r="B196" s="1">
         <v>8</v>
       </c>
+      <c r="E196">
+        <v>120</v>
+      </c>
+      <c r="F196">
+        <v>70</v>
+      </c>
     </row>
     <row r="197" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
@@ -3267,6 +3441,12 @@
       <c r="B200" s="1">
         <v>8</v>
       </c>
+      <c r="E200">
+        <v>110</v>
+      </c>
+      <c r="F200">
+        <v>64</v>
+      </c>
     </row>
     <row r="201" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
@@ -3275,6 +3455,9 @@
       <c r="B201" s="1">
         <v>8</v>
       </c>
+      <c r="E201">
+        <v>85</v>
+      </c>
     </row>
     <row r="202" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
@@ -3353,7 +3536,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
         <v>32</v>
       </c>
@@ -3364,7 +3547,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
         <v>175</v>
       </c>
@@ -3375,7 +3558,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="1" t="s">
         <v>34</v>
       </c>
@@ -3386,7 +3569,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
         <v>175</v>
       </c>
@@ -3394,7 +3577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
         <v>176</v>
       </c>
@@ -3405,7 +3588,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
         <v>177</v>
       </c>
@@ -3416,7 +3599,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
         <v>178</v>
       </c>
@@ -3427,7 +3610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
         <v>179</v>
       </c>
@@ -3438,15 +3621,21 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B217" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E217">
+        <v>20</v>
+      </c>
+      <c r="F217">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
         <v>180</v>
       </c>
@@ -3454,7 +3643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
         <v>181</v>
       </c>
@@ -3462,7 +3651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
         <v>182</v>
       </c>
@@ -3470,15 +3659,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A221" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B221" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E221">
+        <v>11</v>
+      </c>
+      <c r="F221">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
         <v>184</v>
       </c>
@@ -3486,7 +3681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
         <v>131</v>
       </c>
@@ -3494,23 +3689,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B224" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="E224">
+        <v>35</v>
+      </c>
+      <c r="F224">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B225" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="E225">
+        <v>30</v>
+      </c>
+      <c r="F225">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="1" t="s">
         <v>187</v>
       </c>
@@ -3518,7 +3725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="1" t="s">
         <v>188</v>
       </c>
@@ -3526,7 +3733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A228" s="1" t="s">
         <v>189</v>
       </c>
@@ -3534,23 +3741,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B229" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="E229">
+        <v>45</v>
+      </c>
+      <c r="F229">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B230" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="E230">
+        <v>10</v>
+      </c>
+      <c r="F230">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A231" s="1" t="s">
         <v>140</v>
       </c>
@@ -3558,7 +3777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="2" t="s">
         <v>190</v>
       </c>
@@ -3566,15 +3785,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A233" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B233" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="E233">
+        <v>22</v>
+      </c>
+      <c r="F233">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A234" s="1" t="s">
         <v>128</v>
       </c>
@@ -3582,7 +3807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A235" s="1" t="s">
         <v>192</v>
       </c>
@@ -3590,7 +3815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A236" s="1" t="s">
         <v>193</v>
       </c>
@@ -3598,7 +3823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="1" t="s">
         <v>194</v>
       </c>
@@ -3606,15 +3831,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A238" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B238" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="E238">
+        <v>65</v>
+      </c>
+      <c r="F238">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
         <v>195</v>
       </c>
@@ -3622,7 +3853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A240" s="1" t="s">
         <v>196</v>
       </c>
@@ -4042,6 +4273,12 @@
       <c r="B286" s="1">
         <v>13</v>
       </c>
+      <c r="D286">
+        <v>60</v>
+      </c>
+      <c r="E286">
+        <v>105</v>
+      </c>
     </row>
     <row r="287" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A287" s="1" t="s">
@@ -4059,39 +4296,63 @@
         <v>13</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A289" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B289" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D289">
+        <v>80</v>
+      </c>
+      <c r="E289">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A290" s="1" t="s">
         <v>225</v>
       </c>
       <c r="B290" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D290">
+        <v>50</v>
+      </c>
+      <c r="E290">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A291" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B291" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D291">
+        <v>80</v>
+      </c>
+      <c r="E291">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A292" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B292" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D292">
+        <v>80</v>
+      </c>
+      <c r="E292">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A293" s="1" t="s">
         <v>227</v>
       </c>
@@ -4099,23 +4360,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A294" s="1" t="s">
         <v>228</v>
       </c>
       <c r="B294" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D294">
+        <v>95</v>
+      </c>
+      <c r="E294">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A295" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B295" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D295">
+        <v>90</v>
+      </c>
+      <c r="E295">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A296" s="1" t="s">
         <v>230</v>
       </c>
@@ -4123,15 +4396,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A297" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B297" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D297">
+        <v>75</v>
+      </c>
+      <c r="E297">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A298" s="1" t="s">
         <v>232</v>
       </c>
@@ -4139,31 +4418,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A299" s="1" t="s">
         <v>233</v>
       </c>
       <c r="B299" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D299">
+        <v>80</v>
+      </c>
+      <c r="E299">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A300" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B300" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D300">
+        <v>60</v>
+      </c>
+      <c r="E300">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A301" s="1" t="s">
         <v>234</v>
       </c>
       <c r="B301" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="302" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D301">
+        <v>100</v>
+      </c>
+      <c r="E301">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A302" s="1" t="s">
         <v>235</v>
       </c>
@@ -4171,15 +4468,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A303" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B303" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="304" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="D303">
+        <v>50</v>
+      </c>
+      <c r="E303">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A304" s="1" t="s">
         <v>236</v>
       </c>
@@ -4193,6 +4496,12 @@
       </c>
       <c r="B305" s="1">
         <v>13</v>
+      </c>
+      <c r="D305">
+        <v>110</v>
+      </c>
+      <c r="E305">
+        <v>120</v>
       </c>
     </row>
     <row r="306" spans="1:5" ht="13" x14ac:dyDescent="0.15">

</xml_diff>